<commit_message>
add subtitle using pillow
</commit_message>
<xml_diff>
--- a/Gantt_chart.xlsx
+++ b/Gantt_chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c680cefa49b2057/附件/程式1/Project/ytp-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="11_3C4179B01545E19DD6C385890107473B0B440F85" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{986065AA-6241-4DA9-A008-CAE6FEBCE7B0}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="11_3C4179B01545E19DD6C385890107473B0B440F85" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F0C0916-CAE8-4F56-8252-0F52AA14DC0E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -230,47 +230,6 @@
   </si>
   <si>
     <t>Crawling</t>
-    <phoneticPr fontId="32" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>不同類型用不同網站抓</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(ex. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>人名、地名</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>)</t>
-    </r>
     <phoneticPr fontId="32" type="noConversion"/>
   </si>
   <si>
@@ -1389,19 +1348,22 @@
     <xf numFmtId="0" fontId="36" fillId="10" borderId="9" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="179" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1413,17 +1375,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="179" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -2027,10 +1986,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL32"/>
+  <dimension ref="A1:BL31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A24" zoomScale="106" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A19" zoomScale="106" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2049,66 +2008,66 @@
     <row r="1" spans="1:64" ht="90" customHeight="1" x14ac:dyDescent="1.7">
       <c r="A1" s="14"/>
       <c r="B1" s="96" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" s="18"/>
       <c r="D1" s="19"/>
       <c r="E1" s="20"/>
       <c r="F1" s="21"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="120" t="s">
+      <c r="I1" s="121" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="121"/>
-      <c r="K1" s="121"/>
-      <c r="L1" s="121"/>
-      <c r="M1" s="121"/>
-      <c r="N1" s="121"/>
-      <c r="O1" s="121"/>
+      <c r="J1" s="122"/>
+      <c r="K1" s="122"/>
+      <c r="L1" s="122"/>
+      <c r="M1" s="122"/>
+      <c r="N1" s="122"/>
+      <c r="O1" s="122"/>
       <c r="P1" s="24"/>
-      <c r="Q1" s="119">
+      <c r="Q1" s="120">
         <v>45287</v>
       </c>
-      <c r="R1" s="118"/>
-      <c r="S1" s="118"/>
-      <c r="T1" s="118"/>
-      <c r="U1" s="118"/>
-      <c r="V1" s="118"/>
-      <c r="W1" s="118"/>
-      <c r="X1" s="118"/>
-      <c r="Y1" s="118"/>
-      <c r="Z1" s="118"/>
+      <c r="R1" s="119"/>
+      <c r="S1" s="119"/>
+      <c r="T1" s="119"/>
+      <c r="U1" s="119"/>
+      <c r="V1" s="119"/>
+      <c r="W1" s="119"/>
+      <c r="X1" s="119"/>
+      <c r="Y1" s="119"/>
+      <c r="Z1" s="119"/>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B2" s="94" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="95"/>
       <c r="D2" s="22"/>
       <c r="E2" s="23"/>
       <c r="F2" s="22"/>
-      <c r="I2" s="120" t="s">
+      <c r="I2" s="121" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="121"/>
-      <c r="K2" s="121"/>
-      <c r="L2" s="121"/>
-      <c r="M2" s="121"/>
-      <c r="N2" s="121"/>
-      <c r="O2" s="121"/>
+      <c r="J2" s="122"/>
+      <c r="K2" s="122"/>
+      <c r="L2" s="122"/>
+      <c r="M2" s="122"/>
+      <c r="N2" s="122"/>
+      <c r="O2" s="122"/>
       <c r="P2" s="24"/>
-      <c r="Q2" s="117">
+      <c r="Q2" s="118">
         <v>1</v>
       </c>
-      <c r="R2" s="118"/>
-      <c r="S2" s="118"/>
-      <c r="T2" s="118"/>
-      <c r="U2" s="118"/>
-      <c r="V2" s="118"/>
-      <c r="W2" s="118"/>
-      <c r="X2" s="118"/>
-      <c r="Y2" s="118"/>
-      <c r="Z2" s="118"/>
+      <c r="R2" s="119"/>
+      <c r="S2" s="119"/>
+      <c r="T2" s="119"/>
+      <c r="U2" s="119"/>
+      <c r="V2" s="119"/>
+      <c r="W2" s="119"/>
+      <c r="X2" s="119"/>
+      <c r="Y2" s="119"/>
+      <c r="Z2" s="119"/>
     </row>
     <row r="3" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13"/>
@@ -2124,102 +2083,102 @@
         <v>13</v>
       </c>
       <c r="E4" s="30"/>
-      <c r="I4" s="114">
+      <c r="I4" s="125">
         <f>I5</f>
         <v>45285</v>
       </c>
-      <c r="J4" s="112"/>
-      <c r="K4" s="112"/>
-      <c r="L4" s="112"/>
-      <c r="M4" s="112"/>
-      <c r="N4" s="112"/>
-      <c r="O4" s="112"/>
-      <c r="P4" s="112">
+      <c r="J4" s="123"/>
+      <c r="K4" s="123"/>
+      <c r="L4" s="123"/>
+      <c r="M4" s="123"/>
+      <c r="N4" s="123"/>
+      <c r="O4" s="123"/>
+      <c r="P4" s="123">
         <f>P5</f>
         <v>45292</v>
       </c>
-      <c r="Q4" s="112"/>
-      <c r="R4" s="112"/>
-      <c r="S4" s="112"/>
-      <c r="T4" s="112"/>
-      <c r="U4" s="112"/>
-      <c r="V4" s="112"/>
-      <c r="W4" s="112">
+      <c r="Q4" s="123"/>
+      <c r="R4" s="123"/>
+      <c r="S4" s="123"/>
+      <c r="T4" s="123"/>
+      <c r="U4" s="123"/>
+      <c r="V4" s="123"/>
+      <c r="W4" s="123">
         <f>W5</f>
         <v>45299</v>
       </c>
-      <c r="X4" s="112"/>
-      <c r="Y4" s="112"/>
-      <c r="Z4" s="112"/>
-      <c r="AA4" s="112"/>
-      <c r="AB4" s="112"/>
-      <c r="AC4" s="112"/>
-      <c r="AD4" s="112">
+      <c r="X4" s="123"/>
+      <c r="Y4" s="123"/>
+      <c r="Z4" s="123"/>
+      <c r="AA4" s="123"/>
+      <c r="AB4" s="123"/>
+      <c r="AC4" s="123"/>
+      <c r="AD4" s="123">
         <f>AD5</f>
         <v>45306</v>
       </c>
-      <c r="AE4" s="112"/>
-      <c r="AF4" s="112"/>
-      <c r="AG4" s="112"/>
-      <c r="AH4" s="112"/>
-      <c r="AI4" s="112"/>
-      <c r="AJ4" s="112"/>
-      <c r="AK4" s="112">
+      <c r="AE4" s="123"/>
+      <c r="AF4" s="123"/>
+      <c r="AG4" s="123"/>
+      <c r="AH4" s="123"/>
+      <c r="AI4" s="123"/>
+      <c r="AJ4" s="123"/>
+      <c r="AK4" s="123">
         <f>AK5</f>
         <v>45313</v>
       </c>
-      <c r="AL4" s="112"/>
-      <c r="AM4" s="112"/>
-      <c r="AN4" s="112"/>
-      <c r="AO4" s="112"/>
-      <c r="AP4" s="112"/>
-      <c r="AQ4" s="112"/>
-      <c r="AR4" s="112">
+      <c r="AL4" s="123"/>
+      <c r="AM4" s="123"/>
+      <c r="AN4" s="123"/>
+      <c r="AO4" s="123"/>
+      <c r="AP4" s="123"/>
+      <c r="AQ4" s="123"/>
+      <c r="AR4" s="123">
         <f>AR5</f>
         <v>45320</v>
       </c>
-      <c r="AS4" s="112"/>
-      <c r="AT4" s="112"/>
-      <c r="AU4" s="112"/>
-      <c r="AV4" s="112"/>
-      <c r="AW4" s="112"/>
-      <c r="AX4" s="112"/>
-      <c r="AY4" s="112">
+      <c r="AS4" s="123"/>
+      <c r="AT4" s="123"/>
+      <c r="AU4" s="123"/>
+      <c r="AV4" s="123"/>
+      <c r="AW4" s="123"/>
+      <c r="AX4" s="123"/>
+      <c r="AY4" s="123">
         <f>AY5</f>
         <v>45327</v>
       </c>
-      <c r="AZ4" s="112"/>
-      <c r="BA4" s="112"/>
-      <c r="BB4" s="112"/>
-      <c r="BC4" s="112"/>
-      <c r="BD4" s="112"/>
-      <c r="BE4" s="112"/>
-      <c r="BF4" s="112">
+      <c r="AZ4" s="123"/>
+      <c r="BA4" s="123"/>
+      <c r="BB4" s="123"/>
+      <c r="BC4" s="123"/>
+      <c r="BD4" s="123"/>
+      <c r="BE4" s="123"/>
+      <c r="BF4" s="123">
         <f>BF5</f>
         <v>45334</v>
       </c>
-      <c r="BG4" s="112"/>
-      <c r="BH4" s="112"/>
-      <c r="BI4" s="112"/>
-      <c r="BJ4" s="112"/>
-      <c r="BK4" s="112"/>
-      <c r="BL4" s="113"/>
+      <c r="BG4" s="123"/>
+      <c r="BH4" s="123"/>
+      <c r="BI4" s="123"/>
+      <c r="BJ4" s="123"/>
+      <c r="BK4" s="123"/>
+      <c r="BL4" s="124"/>
     </row>
     <row r="5" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="122"/>
-      <c r="B5" s="123" t="s">
+      <c r="A5" s="112"/>
+      <c r="B5" s="113" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="125" t="s">
+      <c r="C5" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="115" t="s">
+      <c r="D5" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="115" t="s">
+      <c r="E5" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="115" t="s">
+      <c r="F5" s="117" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="31">
@@ -2448,8 +2407,8 @@
       </c>
     </row>
     <row r="6" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="122"/>
-      <c r="B6" s="124"/>
+      <c r="A6" s="112"/>
+      <c r="B6" s="114"/>
       <c r="C6" s="116"/>
       <c r="D6" s="116"/>
       <c r="E6" s="116"/>
@@ -2752,7 +2711,7 @@
     <row r="8" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="14"/>
       <c r="B8" s="40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="41"/>
       <c r="D8" s="42"/>
@@ -2760,7 +2719,7 @@
       <c r="F8" s="44"/>
       <c r="G8" s="17"/>
       <c r="H8" s="5" t="str">
-        <f t="shared" ref="H8:H29" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H28" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="45"/>
@@ -3143,7 +3102,7 @@
     <row r="13" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="13"/>
       <c r="B13" s="51" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" s="52" t="s">
         <v>25</v>
@@ -3220,7 +3179,7 @@
     <row r="14" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="13"/>
       <c r="B14" s="107" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="52" t="s">
         <v>25</v>
@@ -3313,27 +3272,27 @@
       </c>
     </row>
     <row r="16" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="14"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="108" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C16" s="61" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D16" s="62">
         <v>0</v>
       </c>
       <c r="E16" s="63">
-        <v>45299</v>
+        <v>45301</v>
       </c>
       <c r="F16" s="63">
-        <f>E16+1</f>
-        <v>45300</v>
+        <f>E16+13</f>
+        <v>45314</v>
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="5">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="I16" s="50"/>
       <c r="J16" s="50"/>
@@ -3347,8 +3306,8 @@
       <c r="R16" s="50"/>
       <c r="S16" s="50"/>
       <c r="T16" s="50"/>
-      <c r="U16" s="50"/>
-      <c r="V16" s="50"/>
+      <c r="U16" s="55"/>
+      <c r="V16" s="55"/>
       <c r="W16" s="50"/>
       <c r="X16" s="50"/>
       <c r="Y16" s="50"/>
@@ -3394,162 +3353,162 @@
     </row>
     <row r="17" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="13"/>
-      <c r="B17" s="108" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="61" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="62">
-        <v>0</v>
-      </c>
-      <c r="E17" s="63">
-        <v>45301</v>
-      </c>
-      <c r="F17" s="63">
-        <f>E17+13</f>
-        <v>45314</v>
-      </c>
+      <c r="B17" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="65"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="68"/>
       <c r="G17" s="17"/>
-      <c r="H17" s="5">
+      <c r="H17" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>14</v>
-      </c>
-      <c r="I17" s="50"/>
-      <c r="J17" s="50"/>
-      <c r="K17" s="50"/>
-      <c r="L17" s="50"/>
-      <c r="M17" s="50"/>
-      <c r="N17" s="50"/>
-      <c r="O17" s="50"/>
-      <c r="P17" s="50"/>
-      <c r="Q17" s="50"/>
-      <c r="R17" s="50"/>
-      <c r="S17" s="50"/>
-      <c r="T17" s="50"/>
-      <c r="U17" s="55"/>
-      <c r="V17" s="55"/>
-      <c r="W17" s="50"/>
-      <c r="X17" s="50"/>
-      <c r="Y17" s="50"/>
-      <c r="Z17" s="50"/>
-      <c r="AA17" s="50"/>
-      <c r="AB17" s="50"/>
-      <c r="AC17" s="50"/>
-      <c r="AD17" s="50"/>
-      <c r="AE17" s="50"/>
-      <c r="AF17" s="50"/>
-      <c r="AG17" s="50"/>
-      <c r="AH17" s="50"/>
-      <c r="AI17" s="50"/>
-      <c r="AJ17" s="50"/>
-      <c r="AK17" s="50"/>
-      <c r="AL17" s="50"/>
-      <c r="AM17" s="50"/>
-      <c r="AN17" s="50"/>
-      <c r="AO17" s="50"/>
-      <c r="AP17" s="50"/>
-      <c r="AQ17" s="50"/>
-      <c r="AR17" s="50"/>
-      <c r="AS17" s="50"/>
-      <c r="AT17" s="50"/>
-      <c r="AU17" s="50"/>
-      <c r="AV17" s="50"/>
-      <c r="AW17" s="50"/>
-      <c r="AX17" s="50"/>
-      <c r="AY17" s="50"/>
-      <c r="AZ17" s="50"/>
-      <c r="BA17" s="50"/>
-      <c r="BB17" s="50"/>
-      <c r="BC17" s="50"/>
-      <c r="BD17" s="50"/>
-      <c r="BE17" s="50"/>
-      <c r="BF17" s="50"/>
-      <c r="BG17" s="50"/>
-      <c r="BH17" s="50"/>
-      <c r="BI17" s="50"/>
-      <c r="BJ17" s="50"/>
-      <c r="BK17" s="50"/>
-      <c r="BL17" s="50"/>
+        <v/>
+      </c>
+      <c r="I17" s="69"/>
+      <c r="J17" s="69"/>
+      <c r="K17" s="69"/>
+      <c r="L17" s="69"/>
+      <c r="M17" s="69"/>
+      <c r="N17" s="69"/>
+      <c r="O17" s="69"/>
+      <c r="P17" s="69"/>
+      <c r="Q17" s="69"/>
+      <c r="R17" s="69"/>
+      <c r="S17" s="69"/>
+      <c r="T17" s="69"/>
+      <c r="U17" s="69"/>
+      <c r="V17" s="69"/>
+      <c r="W17" s="69"/>
+      <c r="X17" s="69"/>
+      <c r="Y17" s="69"/>
+      <c r="Z17" s="69"/>
+      <c r="AA17" s="69"/>
+      <c r="AB17" s="69"/>
+      <c r="AC17" s="69"/>
+      <c r="AD17" s="69"/>
+      <c r="AE17" s="69"/>
+      <c r="AF17" s="69"/>
+      <c r="AG17" s="69"/>
+      <c r="AH17" s="69"/>
+      <c r="AI17" s="69"/>
+      <c r="AJ17" s="69"/>
+      <c r="AK17" s="69"/>
+      <c r="AL17" s="69"/>
+      <c r="AM17" s="69"/>
+      <c r="AN17" s="69"/>
+      <c r="AO17" s="69"/>
+      <c r="AP17" s="69"/>
+      <c r="AQ17" s="69"/>
+      <c r="AR17" s="69"/>
+      <c r="AS17" s="69"/>
+      <c r="AT17" s="69"/>
+      <c r="AU17" s="69"/>
+      <c r="AV17" s="69"/>
+      <c r="AW17" s="69"/>
+      <c r="AX17" s="69"/>
+      <c r="AY17" s="69"/>
+      <c r="AZ17" s="69"/>
+      <c r="BA17" s="69"/>
+      <c r="BB17" s="69"/>
+      <c r="BC17" s="69"/>
+      <c r="BD17" s="69"/>
+      <c r="BE17" s="69"/>
+      <c r="BF17" s="69"/>
+      <c r="BG17" s="69"/>
+      <c r="BH17" s="69"/>
+      <c r="BI17" s="69"/>
+      <c r="BJ17" s="69"/>
+      <c r="BK17" s="69"/>
+      <c r="BL17" s="69"/>
     </row>
     <row r="18" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="13"/>
-      <c r="B18" s="64" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="65"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="68"/>
+      <c r="B18" s="109" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="71" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="72">
+        <v>1</v>
+      </c>
+      <c r="E18" s="73">
+        <v>45301</v>
+      </c>
+      <c r="F18" s="73">
+        <f>E18+6</f>
+        <v>45307</v>
+      </c>
       <c r="G18" s="17"/>
-      <c r="H18" s="5" t="str">
+      <c r="H18" s="5">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I18" s="69"/>
-      <c r="J18" s="69"/>
-      <c r="K18" s="69"/>
-      <c r="L18" s="69"/>
-      <c r="M18" s="69"/>
-      <c r="N18" s="69"/>
-      <c r="O18" s="69"/>
-      <c r="P18" s="69"/>
-      <c r="Q18" s="69"/>
-      <c r="R18" s="69"/>
-      <c r="S18" s="69"/>
-      <c r="T18" s="69"/>
-      <c r="U18" s="69"/>
-      <c r="V18" s="69"/>
-      <c r="W18" s="69"/>
-      <c r="X18" s="69"/>
-      <c r="Y18" s="69"/>
-      <c r="Z18" s="69"/>
-      <c r="AA18" s="69"/>
-      <c r="AB18" s="69"/>
-      <c r="AC18" s="69"/>
-      <c r="AD18" s="69"/>
-      <c r="AE18" s="69"/>
-      <c r="AF18" s="69"/>
-      <c r="AG18" s="69"/>
-      <c r="AH18" s="69"/>
-      <c r="AI18" s="69"/>
-      <c r="AJ18" s="69"/>
-      <c r="AK18" s="69"/>
-      <c r="AL18" s="69"/>
-      <c r="AM18" s="69"/>
-      <c r="AN18" s="69"/>
-      <c r="AO18" s="69"/>
-      <c r="AP18" s="69"/>
-      <c r="AQ18" s="69"/>
-      <c r="AR18" s="69"/>
-      <c r="AS18" s="69"/>
-      <c r="AT18" s="69"/>
-      <c r="AU18" s="69"/>
-      <c r="AV18" s="69"/>
-      <c r="AW18" s="69"/>
-      <c r="AX18" s="69"/>
-      <c r="AY18" s="69"/>
-      <c r="AZ18" s="69"/>
-      <c r="BA18" s="69"/>
-      <c r="BB18" s="69"/>
-      <c r="BC18" s="69"/>
-      <c r="BD18" s="69"/>
-      <c r="BE18" s="69"/>
-      <c r="BF18" s="69"/>
-      <c r="BG18" s="69"/>
-      <c r="BH18" s="69"/>
-      <c r="BI18" s="69"/>
-      <c r="BJ18" s="69"/>
-      <c r="BK18" s="69"/>
-      <c r="BL18" s="69"/>
+        <v>7</v>
+      </c>
+      <c r="I18" s="50"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="50"/>
+      <c r="L18" s="50"/>
+      <c r="M18" s="50"/>
+      <c r="N18" s="50"/>
+      <c r="O18" s="50"/>
+      <c r="P18" s="50"/>
+      <c r="Q18" s="50"/>
+      <c r="R18" s="50"/>
+      <c r="S18" s="50"/>
+      <c r="T18" s="50"/>
+      <c r="U18" s="50"/>
+      <c r="V18" s="50"/>
+      <c r="W18" s="50"/>
+      <c r="X18" s="50"/>
+      <c r="Y18" s="50"/>
+      <c r="Z18" s="50"/>
+      <c r="AA18" s="50"/>
+      <c r="AB18" s="50"/>
+      <c r="AC18" s="50"/>
+      <c r="AD18" s="50"/>
+      <c r="AE18" s="50"/>
+      <c r="AF18" s="50"/>
+      <c r="AG18" s="50"/>
+      <c r="AH18" s="50"/>
+      <c r="AI18" s="50"/>
+      <c r="AJ18" s="50"/>
+      <c r="AK18" s="50"/>
+      <c r="AL18" s="50"/>
+      <c r="AM18" s="50"/>
+      <c r="AN18" s="50"/>
+      <c r="AO18" s="50"/>
+      <c r="AP18" s="50"/>
+      <c r="AQ18" s="50"/>
+      <c r="AR18" s="50"/>
+      <c r="AS18" s="50"/>
+      <c r="AT18" s="50"/>
+      <c r="AU18" s="50"/>
+      <c r="AV18" s="50"/>
+      <c r="AW18" s="50"/>
+      <c r="AX18" s="50"/>
+      <c r="AY18" s="50"/>
+      <c r="AZ18" s="50"/>
+      <c r="BA18" s="50"/>
+      <c r="BB18" s="50"/>
+      <c r="BC18" s="50"/>
+      <c r="BD18" s="50"/>
+      <c r="BE18" s="50"/>
+      <c r="BF18" s="50"/>
+      <c r="BG18" s="50"/>
+      <c r="BH18" s="50"/>
+      <c r="BI18" s="50"/>
+      <c r="BJ18" s="50"/>
+      <c r="BK18" s="50"/>
+      <c r="BL18" s="50"/>
     </row>
     <row r="19" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="13"/>
-      <c r="B19" s="109" t="s">
-        <v>36</v>
+      <c r="B19" s="110" t="s">
+        <v>45</v>
       </c>
       <c r="C19" s="71" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19" s="72">
         <v>0</v>
@@ -3558,14 +3517,11 @@
         <v>45301</v>
       </c>
       <c r="F19" s="73">
-        <f>E19+6</f>
-        <v>45307</v>
+        <f>E19+13</f>
+        <v>45314</v>
       </c>
       <c r="G19" s="17"/>
-      <c r="H19" s="5">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
+      <c r="H19" s="5"/>
       <c r="I19" s="50"/>
       <c r="J19" s="50"/>
       <c r="K19" s="50"/>
@@ -3629,20 +3585,22 @@
         <v>46</v>
       </c>
       <c r="C20" s="71" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" s="72">
         <v>0</v>
       </c>
       <c r="E20" s="73">
-        <v>45301</v>
+        <v>45319</v>
       </c>
       <c r="F20" s="73">
-        <f>E20+13</f>
-        <v>45314</v>
+        <v>45329</v>
       </c>
       <c r="G20" s="17"/>
-      <c r="H20" s="5"/>
+      <c r="H20" s="5">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
       <c r="I20" s="50"/>
       <c r="J20" s="50"/>
       <c r="K20" s="50"/>
@@ -3702,25 +3660,25 @@
     </row>
     <row r="21" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="13"/>
-      <c r="B21" s="110" t="s">
-        <v>47</v>
+      <c r="B21" s="70" t="s">
+        <v>40</v>
       </c>
       <c r="C21" s="71" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D21" s="72">
         <v>0</v>
       </c>
       <c r="E21" s="73">
-        <v>45319</v>
+        <v>45337</v>
       </c>
       <c r="F21" s="73">
-        <v>45329</v>
+        <v>45345</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="5">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I21" s="50"/>
       <c r="J21" s="50"/>
@@ -3781,153 +3739,154 @@
     </row>
     <row r="22" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13"/>
-      <c r="B22" s="70" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="71" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="72">
-        <v>0</v>
-      </c>
-      <c r="E22" s="73">
-        <v>45337</v>
-      </c>
-      <c r="F22" s="73">
-        <v>45345</v>
-      </c>
+      <c r="B22" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="75"/>
+      <c r="D22" s="76"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="78"/>
       <c r="G22" s="17"/>
-      <c r="H22" s="5">
+      <c r="H22" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>9</v>
-      </c>
-      <c r="I22" s="50"/>
-      <c r="J22" s="50"/>
-      <c r="K22" s="50"/>
-      <c r="L22" s="50"/>
-      <c r="M22" s="50"/>
-      <c r="N22" s="50"/>
-      <c r="O22" s="50"/>
-      <c r="P22" s="50"/>
-      <c r="Q22" s="50"/>
-      <c r="R22" s="50"/>
-      <c r="S22" s="50"/>
-      <c r="T22" s="50"/>
-      <c r="U22" s="50"/>
-      <c r="V22" s="50"/>
-      <c r="W22" s="50"/>
-      <c r="X22" s="50"/>
-      <c r="Y22" s="50"/>
-      <c r="Z22" s="50"/>
-      <c r="AA22" s="50"/>
-      <c r="AB22" s="50"/>
-      <c r="AC22" s="50"/>
-      <c r="AD22" s="50"/>
-      <c r="AE22" s="50"/>
-      <c r="AF22" s="50"/>
-      <c r="AG22" s="50"/>
-      <c r="AH22" s="50"/>
-      <c r="AI22" s="50"/>
-      <c r="AJ22" s="50"/>
-      <c r="AK22" s="50"/>
-      <c r="AL22" s="50"/>
-      <c r="AM22" s="50"/>
-      <c r="AN22" s="50"/>
-      <c r="AO22" s="50"/>
-      <c r="AP22" s="50"/>
-      <c r="AQ22" s="50"/>
-      <c r="AR22" s="50"/>
-      <c r="AS22" s="50"/>
-      <c r="AT22" s="50"/>
-      <c r="AU22" s="50"/>
-      <c r="AV22" s="50"/>
-      <c r="AW22" s="50"/>
-      <c r="AX22" s="50"/>
-      <c r="AY22" s="50"/>
-      <c r="AZ22" s="50"/>
-      <c r="BA22" s="50"/>
-      <c r="BB22" s="50"/>
-      <c r="BC22" s="50"/>
-      <c r="BD22" s="50"/>
-      <c r="BE22" s="50"/>
-      <c r="BF22" s="50"/>
-      <c r="BG22" s="50"/>
-      <c r="BH22" s="50"/>
-      <c r="BI22" s="50"/>
-      <c r="BJ22" s="50"/>
-      <c r="BK22" s="50"/>
-      <c r="BL22" s="50"/>
+        <v/>
+      </c>
+      <c r="I22" s="79"/>
+      <c r="J22" s="79"/>
+      <c r="K22" s="79"/>
+      <c r="L22" s="79"/>
+      <c r="M22" s="79"/>
+      <c r="N22" s="79"/>
+      <c r="O22" s="79"/>
+      <c r="P22" s="79"/>
+      <c r="Q22" s="79"/>
+      <c r="R22" s="79"/>
+      <c r="S22" s="79"/>
+      <c r="T22" s="79"/>
+      <c r="U22" s="79"/>
+      <c r="V22" s="79"/>
+      <c r="W22" s="79"/>
+      <c r="X22" s="79"/>
+      <c r="Y22" s="79"/>
+      <c r="Z22" s="79"/>
+      <c r="AA22" s="79"/>
+      <c r="AB22" s="79"/>
+      <c r="AC22" s="79"/>
+      <c r="AD22" s="79"/>
+      <c r="AE22" s="79"/>
+      <c r="AF22" s="79"/>
+      <c r="AG22" s="79"/>
+      <c r="AH22" s="79"/>
+      <c r="AI22" s="79"/>
+      <c r="AJ22" s="79"/>
+      <c r="AK22" s="79"/>
+      <c r="AL22" s="79"/>
+      <c r="AM22" s="79"/>
+      <c r="AN22" s="79"/>
+      <c r="AO22" s="79"/>
+      <c r="AP22" s="79"/>
+      <c r="AQ22" s="79"/>
+      <c r="AR22" s="79"/>
+      <c r="AS22" s="79"/>
+      <c r="AT22" s="79"/>
+      <c r="AU22" s="79"/>
+      <c r="AV22" s="79"/>
+      <c r="AW22" s="79"/>
+      <c r="AX22" s="79"/>
+      <c r="AY22" s="79"/>
+      <c r="AZ22" s="79"/>
+      <c r="BA22" s="79"/>
+      <c r="BB22" s="79"/>
+      <c r="BC22" s="79"/>
+      <c r="BD22" s="79"/>
+      <c r="BE22" s="79"/>
+      <c r="BF22" s="79"/>
+      <c r="BG22" s="79"/>
+      <c r="BH22" s="79"/>
+      <c r="BI22" s="79"/>
+      <c r="BJ22" s="79"/>
+      <c r="BK22" s="79"/>
+      <c r="BL22" s="79"/>
     </row>
     <row r="23" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="13"/>
-      <c r="B23" s="74" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="75"/>
-      <c r="D23" s="76"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="78"/>
+      <c r="B23" s="111" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="82">
+        <v>0</v>
+      </c>
+      <c r="E23" s="83">
+        <v>45308</v>
+      </c>
+      <c r="F23" s="83">
+        <f>E23+13</f>
+        <v>45321</v>
+      </c>
       <c r="G23" s="17"/>
-      <c r="H23" s="5" t="str">
+      <c r="H23" s="5">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I23" s="79"/>
-      <c r="J23" s="79"/>
-      <c r="K23" s="79"/>
-      <c r="L23" s="79"/>
-      <c r="M23" s="79"/>
-      <c r="N23" s="79"/>
-      <c r="O23" s="79"/>
-      <c r="P23" s="79"/>
-      <c r="Q23" s="79"/>
-      <c r="R23" s="79"/>
-      <c r="S23" s="79"/>
-      <c r="T23" s="79"/>
-      <c r="U23" s="79"/>
-      <c r="V23" s="79"/>
-      <c r="W23" s="79"/>
-      <c r="X23" s="79"/>
-      <c r="Y23" s="79"/>
-      <c r="Z23" s="79"/>
-      <c r="AA23" s="79"/>
-      <c r="AB23" s="79"/>
-      <c r="AC23" s="79"/>
-      <c r="AD23" s="79"/>
-      <c r="AE23" s="79"/>
-      <c r="AF23" s="79"/>
-      <c r="AG23" s="79"/>
-      <c r="AH23" s="79"/>
-      <c r="AI23" s="79"/>
-      <c r="AJ23" s="79"/>
-      <c r="AK23" s="79"/>
-      <c r="AL23" s="79"/>
-      <c r="AM23" s="79"/>
-      <c r="AN23" s="79"/>
-      <c r="AO23" s="79"/>
-      <c r="AP23" s="79"/>
-      <c r="AQ23" s="79"/>
-      <c r="AR23" s="79"/>
-      <c r="AS23" s="79"/>
-      <c r="AT23" s="79"/>
-      <c r="AU23" s="79"/>
-      <c r="AV23" s="79"/>
-      <c r="AW23" s="79"/>
-      <c r="AX23" s="79"/>
-      <c r="AY23" s="79"/>
-      <c r="AZ23" s="79"/>
-      <c r="BA23" s="79"/>
-      <c r="BB23" s="79"/>
-      <c r="BC23" s="79"/>
-      <c r="BD23" s="79"/>
-      <c r="BE23" s="79"/>
-      <c r="BF23" s="79"/>
-      <c r="BG23" s="79"/>
-      <c r="BH23" s="79"/>
-      <c r="BI23" s="79"/>
-      <c r="BJ23" s="79"/>
-      <c r="BK23" s="79"/>
-      <c r="BL23" s="79"/>
+        <v>14</v>
+      </c>
+      <c r="I23" s="50"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="50"/>
+      <c r="P23" s="50"/>
+      <c r="Q23" s="50"/>
+      <c r="R23" s="50"/>
+      <c r="S23" s="50"/>
+      <c r="T23" s="50"/>
+      <c r="U23" s="50"/>
+      <c r="V23" s="50"/>
+      <c r="W23" s="50"/>
+      <c r="X23" s="50"/>
+      <c r="Y23" s="50"/>
+      <c r="Z23" s="50"/>
+      <c r="AA23" s="50"/>
+      <c r="AB23" s="50"/>
+      <c r="AC23" s="50"/>
+      <c r="AD23" s="50"/>
+      <c r="AE23" s="50"/>
+      <c r="AF23" s="50"/>
+      <c r="AG23" s="50"/>
+      <c r="AH23" s="50"/>
+      <c r="AI23" s="50"/>
+      <c r="AJ23" s="50"/>
+      <c r="AK23" s="50"/>
+      <c r="AL23" s="50"/>
+      <c r="AM23" s="50"/>
+      <c r="AN23" s="50"/>
+      <c r="AO23" s="50"/>
+      <c r="AP23" s="50"/>
+      <c r="AQ23" s="50"/>
+      <c r="AR23" s="50"/>
+      <c r="AS23" s="50"/>
+      <c r="AT23" s="50"/>
+      <c r="AU23" s="50"/>
+      <c r="AV23" s="50"/>
+      <c r="AW23" s="50"/>
+      <c r="AX23" s="50"/>
+      <c r="AY23" s="50"/>
+      <c r="AZ23" s="50"/>
+      <c r="BA23" s="50"/>
+      <c r="BB23" s="50"/>
+      <c r="BC23" s="50"/>
+      <c r="BD23" s="50"/>
+      <c r="BE23" s="50"/>
+      <c r="BF23" s="50"/>
+      <c r="BG23" s="50"/>
+      <c r="BH23" s="50"/>
+      <c r="BI23" s="50"/>
+      <c r="BJ23" s="50"/>
+      <c r="BK23" s="50"/>
+      <c r="BL23" s="50"/>
     </row>
     <row r="24" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="13"/>
@@ -3935,17 +3894,17 @@
         <v>43</v>
       </c>
       <c r="C24" s="81" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D24" s="82">
         <v>0</v>
       </c>
       <c r="E24" s="83">
-        <v>45308</v>
+        <v>45322</v>
       </c>
       <c r="F24" s="83">
         <f>E24+13</f>
-        <v>45321</v>
+        <v>45335</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="5">
@@ -4012,25 +3971,26 @@
     <row r="25" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="13"/>
       <c r="B25" s="111" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C25" s="81" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D25" s="82">
         <v>0</v>
       </c>
       <c r="E25" s="83">
-        <v>45322</v>
+        <f>E23+7</f>
+        <v>45315</v>
       </c>
       <c r="F25" s="83">
-        <f>E25+13</f>
-        <v>45335</v>
+        <f>F23</f>
+        <v>45321</v>
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="5">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="I25" s="50"/>
       <c r="J25" s="50"/>
@@ -4091,8 +4051,8 @@
     </row>
     <row r="26" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="13"/>
-      <c r="B26" s="111" t="s">
-        <v>42</v>
+      <c r="B26" s="80" t="s">
+        <v>40</v>
       </c>
       <c r="C26" s="81" t="s">
         <v>25</v>
@@ -4101,17 +4061,17 @@
         <v>0</v>
       </c>
       <c r="E26" s="83">
-        <f>E24+7</f>
-        <v>45315</v>
+        <f>F23+1</f>
+        <v>45322</v>
       </c>
       <c r="F26" s="83">
-        <f>F24</f>
-        <v>45321</v>
+        <f>E26+7</f>
+        <v>45329</v>
       </c>
       <c r="G26" s="17"/>
       <c r="H26" s="5">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I26" s="50"/>
       <c r="J26" s="50"/>
@@ -4172,247 +4132,156 @@
     </row>
     <row r="27" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="13"/>
-      <c r="B27" s="80" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="82">
-        <v>0</v>
-      </c>
-      <c r="E27" s="83">
-        <f>F24+1</f>
-        <v>45322</v>
-      </c>
-      <c r="F27" s="83">
-        <f>E27+7</f>
-        <v>45329</v>
-      </c>
+      <c r="B27" s="84"/>
+      <c r="C27" s="85"/>
+      <c r="D27" s="86"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="87"/>
       <c r="G27" s="17"/>
-      <c r="H27" s="5">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="I27" s="50"/>
-      <c r="J27" s="50"/>
-      <c r="K27" s="50"/>
-      <c r="L27" s="50"/>
-      <c r="M27" s="50"/>
-      <c r="N27" s="50"/>
-      <c r="O27" s="50"/>
-      <c r="P27" s="50"/>
-      <c r="Q27" s="50"/>
-      <c r="R27" s="50"/>
-      <c r="S27" s="50"/>
-      <c r="T27" s="50"/>
-      <c r="U27" s="50"/>
-      <c r="V27" s="50"/>
-      <c r="W27" s="50"/>
-      <c r="X27" s="50"/>
-      <c r="Y27" s="50"/>
-      <c r="Z27" s="50"/>
-      <c r="AA27" s="50"/>
-      <c r="AB27" s="50"/>
-      <c r="AC27" s="50"/>
-      <c r="AD27" s="50"/>
-      <c r="AE27" s="50"/>
-      <c r="AF27" s="50"/>
-      <c r="AG27" s="50"/>
-      <c r="AH27" s="50"/>
-      <c r="AI27" s="50"/>
-      <c r="AJ27" s="50"/>
-      <c r="AK27" s="50"/>
-      <c r="AL27" s="50"/>
-      <c r="AM27" s="50"/>
-      <c r="AN27" s="50"/>
-      <c r="AO27" s="50"/>
-      <c r="AP27" s="50"/>
-      <c r="AQ27" s="50"/>
-      <c r="AR27" s="50"/>
-      <c r="AS27" s="50"/>
-      <c r="AT27" s="50"/>
-      <c r="AU27" s="50"/>
-      <c r="AV27" s="50"/>
-      <c r="AW27" s="50"/>
-      <c r="AX27" s="50"/>
-      <c r="AY27" s="50"/>
-      <c r="AZ27" s="50"/>
-      <c r="BA27" s="50"/>
-      <c r="BB27" s="50"/>
-      <c r="BC27" s="50"/>
-      <c r="BD27" s="50"/>
-      <c r="BE27" s="50"/>
-      <c r="BF27" s="50"/>
-      <c r="BG27" s="50"/>
-      <c r="BH27" s="50"/>
-      <c r="BI27" s="50"/>
-      <c r="BJ27" s="50"/>
-      <c r="BK27" s="50"/>
-      <c r="BL27" s="50"/>
-    </row>
-    <row r="28" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="13"/>
-      <c r="B28" s="84"/>
-      <c r="C28" s="85"/>
-      <c r="D28" s="86"/>
-      <c r="E28" s="87"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="5" t="str">
+      <c r="H27" s="5" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
-      <c r="K28" s="45"/>
-      <c r="L28" s="45"/>
-      <c r="M28" s="45"/>
-      <c r="N28" s="45"/>
-      <c r="O28" s="45"/>
-      <c r="P28" s="45"/>
-      <c r="Q28" s="45"/>
-      <c r="R28" s="45"/>
-      <c r="S28" s="45"/>
-      <c r="T28" s="45"/>
-      <c r="U28" s="45"/>
-      <c r="V28" s="45"/>
-      <c r="W28" s="45"/>
-      <c r="X28" s="45"/>
-      <c r="Y28" s="45"/>
-      <c r="Z28" s="45"/>
-      <c r="AA28" s="45"/>
-      <c r="AB28" s="45"/>
-      <c r="AC28" s="45"/>
-      <c r="AD28" s="45"/>
-      <c r="AE28" s="45"/>
-      <c r="AF28" s="45"/>
-      <c r="AG28" s="45"/>
-      <c r="AH28" s="45"/>
-      <c r="AI28" s="45"/>
-      <c r="AJ28" s="45"/>
-      <c r="AK28" s="45"/>
-      <c r="AL28" s="45"/>
-      <c r="AM28" s="45"/>
-      <c r="AN28" s="45"/>
-      <c r="AO28" s="45"/>
-      <c r="AP28" s="45"/>
-      <c r="AQ28" s="45"/>
-      <c r="AR28" s="45"/>
-      <c r="AS28" s="45"/>
-      <c r="AT28" s="45"/>
-      <c r="AU28" s="45"/>
-      <c r="AV28" s="45"/>
-      <c r="AW28" s="45"/>
-      <c r="AX28" s="45"/>
-      <c r="AY28" s="45"/>
-      <c r="AZ28" s="45"/>
-      <c r="BA28" s="45"/>
-      <c r="BB28" s="45"/>
-      <c r="BC28" s="45"/>
-      <c r="BD28" s="45"/>
-      <c r="BE28" s="45"/>
-      <c r="BF28" s="45"/>
-      <c r="BG28" s="45"/>
-      <c r="BH28" s="45"/>
-      <c r="BI28" s="45"/>
-      <c r="BJ28" s="45"/>
-      <c r="BK28" s="45"/>
-      <c r="BL28" s="45"/>
-    </row>
-    <row r="29" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="14"/>
-      <c r="B29" s="88" t="s">
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="45"/>
+      <c r="L27" s="45"/>
+      <c r="M27" s="45"/>
+      <c r="N27" s="45"/>
+      <c r="O27" s="45"/>
+      <c r="P27" s="45"/>
+      <c r="Q27" s="45"/>
+      <c r="R27" s="45"/>
+      <c r="S27" s="45"/>
+      <c r="T27" s="45"/>
+      <c r="U27" s="45"/>
+      <c r="V27" s="45"/>
+      <c r="W27" s="45"/>
+      <c r="X27" s="45"/>
+      <c r="Y27" s="45"/>
+      <c r="Z27" s="45"/>
+      <c r="AA27" s="45"/>
+      <c r="AB27" s="45"/>
+      <c r="AC27" s="45"/>
+      <c r="AD27" s="45"/>
+      <c r="AE27" s="45"/>
+      <c r="AF27" s="45"/>
+      <c r="AG27" s="45"/>
+      <c r="AH27" s="45"/>
+      <c r="AI27" s="45"/>
+      <c r="AJ27" s="45"/>
+      <c r="AK27" s="45"/>
+      <c r="AL27" s="45"/>
+      <c r="AM27" s="45"/>
+      <c r="AN27" s="45"/>
+      <c r="AO27" s="45"/>
+      <c r="AP27" s="45"/>
+      <c r="AQ27" s="45"/>
+      <c r="AR27" s="45"/>
+      <c r="AS27" s="45"/>
+      <c r="AT27" s="45"/>
+      <c r="AU27" s="45"/>
+      <c r="AV27" s="45"/>
+      <c r="AW27" s="45"/>
+      <c r="AX27" s="45"/>
+      <c r="AY27" s="45"/>
+      <c r="AZ27" s="45"/>
+      <c r="BA27" s="45"/>
+      <c r="BB27" s="45"/>
+      <c r="BC27" s="45"/>
+      <c r="BD27" s="45"/>
+      <c r="BE27" s="45"/>
+      <c r="BF27" s="45"/>
+      <c r="BG27" s="45"/>
+      <c r="BH27" s="45"/>
+      <c r="BI27" s="45"/>
+      <c r="BJ27" s="45"/>
+      <c r="BK27" s="45"/>
+      <c r="BL27" s="45"/>
+    </row>
+    <row r="28" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="14"/>
+      <c r="B28" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="C29" s="89"/>
-      <c r="D29" s="90"/>
-      <c r="E29" s="91"/>
-      <c r="F29" s="92"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="6" t="str">
+      <c r="C28" s="89"/>
+      <c r="D28" s="90"/>
+      <c r="E28" s="91"/>
+      <c r="F28" s="92"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="6" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="I29" s="93"/>
-      <c r="J29" s="93"/>
-      <c r="K29" s="93"/>
-      <c r="L29" s="93"/>
-      <c r="M29" s="93"/>
-      <c r="N29" s="93"/>
-      <c r="O29" s="93"/>
-      <c r="P29" s="93"/>
-      <c r="Q29" s="93"/>
-      <c r="R29" s="93"/>
-      <c r="S29" s="93"/>
-      <c r="T29" s="93"/>
-      <c r="U29" s="93"/>
-      <c r="V29" s="93"/>
-      <c r="W29" s="93"/>
-      <c r="X29" s="93"/>
-      <c r="Y29" s="93"/>
-      <c r="Z29" s="93"/>
-      <c r="AA29" s="93"/>
-      <c r="AB29" s="93"/>
-      <c r="AC29" s="93"/>
-      <c r="AD29" s="93"/>
-      <c r="AE29" s="93"/>
-      <c r="AF29" s="93"/>
-      <c r="AG29" s="93"/>
-      <c r="AH29" s="93"/>
-      <c r="AI29" s="93"/>
-      <c r="AJ29" s="93"/>
-      <c r="AK29" s="93"/>
-      <c r="AL29" s="93"/>
-      <c r="AM29" s="93"/>
-      <c r="AN29" s="93"/>
-      <c r="AO29" s="93"/>
-      <c r="AP29" s="93"/>
-      <c r="AQ29" s="93"/>
-      <c r="AR29" s="93"/>
-      <c r="AS29" s="93"/>
-      <c r="AT29" s="93"/>
-      <c r="AU29" s="93"/>
-      <c r="AV29" s="93"/>
-      <c r="AW29" s="93"/>
-      <c r="AX29" s="93"/>
-      <c r="AY29" s="93"/>
-      <c r="AZ29" s="93"/>
-      <c r="BA29" s="93"/>
-      <c r="BB29" s="93"/>
-      <c r="BC29" s="93"/>
-      <c r="BD29" s="93"/>
-      <c r="BE29" s="93"/>
-      <c r="BF29" s="93"/>
-      <c r="BG29" s="93"/>
-      <c r="BH29" s="93"/>
-      <c r="BI29" s="93"/>
-      <c r="BJ29" s="93"/>
-      <c r="BK29" s="93"/>
-      <c r="BL29" s="93"/>
+      <c r="I28" s="93"/>
+      <c r="J28" s="93"/>
+      <c r="K28" s="93"/>
+      <c r="L28" s="93"/>
+      <c r="M28" s="93"/>
+      <c r="N28" s="93"/>
+      <c r="O28" s="93"/>
+      <c r="P28" s="93"/>
+      <c r="Q28" s="93"/>
+      <c r="R28" s="93"/>
+      <c r="S28" s="93"/>
+      <c r="T28" s="93"/>
+      <c r="U28" s="93"/>
+      <c r="V28" s="93"/>
+      <c r="W28" s="93"/>
+      <c r="X28" s="93"/>
+      <c r="Y28" s="93"/>
+      <c r="Z28" s="93"/>
+      <c r="AA28" s="93"/>
+      <c r="AB28" s="93"/>
+      <c r="AC28" s="93"/>
+      <c r="AD28" s="93"/>
+      <c r="AE28" s="93"/>
+      <c r="AF28" s="93"/>
+      <c r="AG28" s="93"/>
+      <c r="AH28" s="93"/>
+      <c r="AI28" s="93"/>
+      <c r="AJ28" s="93"/>
+      <c r="AK28" s="93"/>
+      <c r="AL28" s="93"/>
+      <c r="AM28" s="93"/>
+      <c r="AN28" s="93"/>
+      <c r="AO28" s="93"/>
+      <c r="AP28" s="93"/>
+      <c r="AQ28" s="93"/>
+      <c r="AR28" s="93"/>
+      <c r="AS28" s="93"/>
+      <c r="AT28" s="93"/>
+      <c r="AU28" s="93"/>
+      <c r="AV28" s="93"/>
+      <c r="AW28" s="93"/>
+      <c r="AX28" s="93"/>
+      <c r="AY28" s="93"/>
+      <c r="AZ28" s="93"/>
+      <c r="BA28" s="93"/>
+      <c r="BB28" s="93"/>
+      <c r="BC28" s="93"/>
+      <c r="BD28" s="93"/>
+      <c r="BE28" s="93"/>
+      <c r="BF28" s="93"/>
+      <c r="BG28" s="93"/>
+      <c r="BH28" s="93"/>
+      <c r="BI28" s="93"/>
+      <c r="BJ28" s="93"/>
+      <c r="BK28" s="93"/>
+      <c r="BL28" s="93"/>
+    </row>
+    <row r="29" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G30" s="3"/>
+      <c r="C30" s="16"/>
+      <c r="F30" s="15"/>
     </row>
     <row r="31" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="16"/>
-      <c r="F31" s="15"/>
-    </row>
-    <row r="32" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="4"/>
+      <c r="C31" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
@@ -4421,9 +4290,19 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <phoneticPr fontId="32" type="noConversion"/>
-  <conditionalFormatting sqref="D7:D29">
+  <conditionalFormatting sqref="D7:D28">
     <cfRule type="dataBar" priority="23">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4445,7 +4324,7 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I16:BL17">
+  <conditionalFormatting sqref="I16:BL16">
     <cfRule type="expression" dxfId="6" priority="4">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4453,7 +4332,7 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I19:BL22">
+  <conditionalFormatting sqref="I18:BL21">
     <cfRule type="expression" dxfId="4" priority="2">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4461,7 +4340,7 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I24:BL27">
+  <conditionalFormatting sqref="I23:BL26">
     <cfRule type="expression" dxfId="2" priority="36">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4469,7 +4348,7 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4:BL27">
+  <conditionalFormatting sqref="I4:BL26">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND(TODAY()&gt;=I$5, TODAY()&lt;J$5)</formula>
     </cfRule>
@@ -4487,9 +4366,9 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="B9 contains the task name.  C9 is the assignee.  D9 is a progress bar that shades based on the number entered into the cell.  _x000a__x000a_E9 contains the start date and F9 contains the end date._x000a__x000a_The Gantt chart will fill in starting in cell I9 based on task dates." sqref="A9" xr:uid="{D870A2F6-6B07-4F5A-A81D-4BCCFADF8796}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Rows 10 through 13 repeat the pattern from row 9. _x000a__x000a_Repeat the instructions from cell A9 for all task rows in this worksheet. _x000a__x000a_Continue entering tasks in cells A10 through A13 or go to cell A14 to learn more." sqref="A10" xr:uid="{872449A7-C3CC-45B6-BA90-B1AAD66BA0E5}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cell B14 contains the Phase 2 sample title. Enter a new title in cell B14._x000a_To delete the phase and work only from tasks, simply delete this row. To remove the phase, simply delete the row. Add tasks to previous phase by entering a new row above this one._x000a_" sqref="A15" xr:uid="{4F48FC41-E335-47F1-87AA-3333A52AD81C}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 3's sample block starts in cell B20." sqref="A18" xr:uid="{956902D1-D3B5-416D-BB69-9362D193BC0A}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 4's sample block starts in cell B26." sqref="A23" xr:uid="{DE54E5DE-526D-4D71-8D03-E99B4AB2FEE5}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Project Schedule. DO NOT enter anything in this row. _x000a_Insert new rows ABOVE this one to continue building out your Project Schedule." sqref="A29" xr:uid="{79B9237E-4DD3-4E0F-8ED6-E0B695A99D96}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 3's sample block starts in cell B20." sqref="A17" xr:uid="{956902D1-D3B5-416D-BB69-9362D193BC0A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 4's sample block starts in cell B26." sqref="A22" xr:uid="{DE54E5DE-526D-4D71-8D03-E99B4AB2FEE5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Project Schedule. DO NOT enter anything in this row. _x000a_Insert new rows ABOVE this one to continue building out your Project Schedule." sqref="A28" xr:uid="{79B9237E-4DD3-4E0F-8ED6-E0B695A99D96}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -4517,7 +4396,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D29</xm:sqref>
+          <xm:sqref>D7:D28</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4671,6 +4550,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4982,15 +4870,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
@@ -5011,6 +4890,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2348D59-3426-404A-A0C5-6456F6613EDB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5031,14 +4918,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
modularize code into main.py in video_v3
</commit_message>
<xml_diff>
--- a/Gantt_chart.xlsx
+++ b/Gantt_chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c680cefa49b2057/附件/程式1/Project/ytp-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="154" documentId="11_3C4179B01545E19DD6C385890107473B0B440F85" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2AAB825-746A-4B7B-8FD4-9EB59C44AD73}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="11_3C4179B01545E19DD6C385890107473B0B440F85" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62B13D6C-BA63-4EEA-BE1C-D882FE220A11}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project schedule" sheetId="11" r:id="rId1"/>
@@ -1348,19 +1348,22 @@
     <xf numFmtId="0" fontId="36" fillId="10" borderId="9" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="179" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1372,17 +1375,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="179" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1776,10 +1776,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1988,24 +1984,24 @@
   </sheetPr>
   <dimension ref="A1:BL31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A5" zoomScale="106" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A10" zoomScale="106" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
-    <col min="7" max="7" width="2.6640625" customWidth="1"/>
+    <col min="1" max="1" width="2.640625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="38.640625" customWidth="1"/>
+    <col min="3" max="3" width="16.640625" customWidth="1"/>
+    <col min="4" max="4" width="10.640625" customWidth="1"/>
+    <col min="5" max="5" width="10.640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.640625" customWidth="1"/>
+    <col min="7" max="7" width="2.640625" customWidth="1"/>
     <col min="8" max="8" width="6" hidden="1" customWidth="1"/>
-    <col min="9" max="65" width="2.6640625" customWidth="1"/>
+    <col min="9" max="65" width="2.640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="90" customHeight="1" x14ac:dyDescent="1.7">
+    <row r="1" spans="1:64" ht="90" customHeight="1" x14ac:dyDescent="1.95">
       <c r="A1" s="14"/>
       <c r="B1" s="96" t="s">
         <v>31</v>
@@ -2015,30 +2011,30 @@
       <c r="E1" s="20"/>
       <c r="F1" s="21"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="120" t="s">
+      <c r="I1" s="121" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="121"/>
-      <c r="K1" s="121"/>
-      <c r="L1" s="121"/>
-      <c r="M1" s="121"/>
-      <c r="N1" s="121"/>
-      <c r="O1" s="121"/>
+      <c r="J1" s="122"/>
+      <c r="K1" s="122"/>
+      <c r="L1" s="122"/>
+      <c r="M1" s="122"/>
+      <c r="N1" s="122"/>
+      <c r="O1" s="122"/>
       <c r="P1" s="24"/>
-      <c r="Q1" s="119">
+      <c r="Q1" s="120">
         <v>45287</v>
       </c>
-      <c r="R1" s="118"/>
-      <c r="S1" s="118"/>
-      <c r="T1" s="118"/>
-      <c r="U1" s="118"/>
-      <c r="V1" s="118"/>
-      <c r="W1" s="118"/>
-      <c r="X1" s="118"/>
-      <c r="Y1" s="118"/>
-      <c r="Z1" s="118"/>
-    </row>
-    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="R1" s="119"/>
+      <c r="S1" s="119"/>
+      <c r="T1" s="119"/>
+      <c r="U1" s="119"/>
+      <c r="V1" s="119"/>
+      <c r="W1" s="119"/>
+      <c r="X1" s="119"/>
+      <c r="Y1" s="119"/>
+      <c r="Z1" s="119"/>
+    </row>
+    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.8">
       <c r="B2" s="94" t="s">
         <v>32</v>
       </c>
@@ -2046,30 +2042,30 @@
       <c r="D2" s="22"/>
       <c r="E2" s="23"/>
       <c r="F2" s="22"/>
-      <c r="I2" s="120" t="s">
+      <c r="I2" s="121" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="121"/>
-      <c r="K2" s="121"/>
-      <c r="L2" s="121"/>
-      <c r="M2" s="121"/>
-      <c r="N2" s="121"/>
-      <c r="O2" s="121"/>
+      <c r="J2" s="122"/>
+      <c r="K2" s="122"/>
+      <c r="L2" s="122"/>
+      <c r="M2" s="122"/>
+      <c r="N2" s="122"/>
+      <c r="O2" s="122"/>
       <c r="P2" s="24"/>
-      <c r="Q2" s="117">
+      <c r="Q2" s="118">
         <v>1</v>
       </c>
-      <c r="R2" s="118"/>
-      <c r="S2" s="118"/>
-      <c r="T2" s="118"/>
-      <c r="U2" s="118"/>
-      <c r="V2" s="118"/>
-      <c r="W2" s="118"/>
-      <c r="X2" s="118"/>
-      <c r="Y2" s="118"/>
-      <c r="Z2" s="118"/>
-    </row>
-    <row r="3" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R2" s="119"/>
+      <c r="S2" s="119"/>
+      <c r="T2" s="119"/>
+      <c r="U2" s="119"/>
+      <c r="V2" s="119"/>
+      <c r="W2" s="119"/>
+      <c r="X2" s="119"/>
+      <c r="Y2" s="119"/>
+      <c r="Z2" s="119"/>
+    </row>
+    <row r="3" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
       <c r="B3" s="25" t="s">
         <v>8</v>
@@ -2077,108 +2073,108 @@
       <c r="D3" s="27"/>
       <c r="E3" s="28"/>
     </row>
-    <row r="4" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14"/>
       <c r="B4" s="29" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="30"/>
-      <c r="I4" s="114">
+      <c r="I4" s="125">
         <f>I5</f>
         <v>45285</v>
       </c>
-      <c r="J4" s="112"/>
-      <c r="K4" s="112"/>
-      <c r="L4" s="112"/>
-      <c r="M4" s="112"/>
-      <c r="N4" s="112"/>
-      <c r="O4" s="112"/>
-      <c r="P4" s="112">
+      <c r="J4" s="123"/>
+      <c r="K4" s="123"/>
+      <c r="L4" s="123"/>
+      <c r="M4" s="123"/>
+      <c r="N4" s="123"/>
+      <c r="O4" s="123"/>
+      <c r="P4" s="123">
         <f>P5</f>
         <v>45292</v>
       </c>
-      <c r="Q4" s="112"/>
-      <c r="R4" s="112"/>
-      <c r="S4" s="112"/>
-      <c r="T4" s="112"/>
-      <c r="U4" s="112"/>
-      <c r="V4" s="112"/>
-      <c r="W4" s="112">
+      <c r="Q4" s="123"/>
+      <c r="R4" s="123"/>
+      <c r="S4" s="123"/>
+      <c r="T4" s="123"/>
+      <c r="U4" s="123"/>
+      <c r="V4" s="123"/>
+      <c r="W4" s="123">
         <f>W5</f>
         <v>45299</v>
       </c>
-      <c r="X4" s="112"/>
-      <c r="Y4" s="112"/>
-      <c r="Z4" s="112"/>
-      <c r="AA4" s="112"/>
-      <c r="AB4" s="112"/>
-      <c r="AC4" s="112"/>
-      <c r="AD4" s="112">
+      <c r="X4" s="123"/>
+      <c r="Y4" s="123"/>
+      <c r="Z4" s="123"/>
+      <c r="AA4" s="123"/>
+      <c r="AB4" s="123"/>
+      <c r="AC4" s="123"/>
+      <c r="AD4" s="123">
         <f>AD5</f>
         <v>45306</v>
       </c>
-      <c r="AE4" s="112"/>
-      <c r="AF4" s="112"/>
-      <c r="AG4" s="112"/>
-      <c r="AH4" s="112"/>
-      <c r="AI4" s="112"/>
-      <c r="AJ4" s="112"/>
-      <c r="AK4" s="112">
+      <c r="AE4" s="123"/>
+      <c r="AF4" s="123"/>
+      <c r="AG4" s="123"/>
+      <c r="AH4" s="123"/>
+      <c r="AI4" s="123"/>
+      <c r="AJ4" s="123"/>
+      <c r="AK4" s="123">
         <f>AK5</f>
         <v>45313</v>
       </c>
-      <c r="AL4" s="112"/>
-      <c r="AM4" s="112"/>
-      <c r="AN4" s="112"/>
-      <c r="AO4" s="112"/>
-      <c r="AP4" s="112"/>
-      <c r="AQ4" s="112"/>
-      <c r="AR4" s="112">
+      <c r="AL4" s="123"/>
+      <c r="AM4" s="123"/>
+      <c r="AN4" s="123"/>
+      <c r="AO4" s="123"/>
+      <c r="AP4" s="123"/>
+      <c r="AQ4" s="123"/>
+      <c r="AR4" s="123">
         <f>AR5</f>
         <v>45320</v>
       </c>
-      <c r="AS4" s="112"/>
-      <c r="AT4" s="112"/>
-      <c r="AU4" s="112"/>
-      <c r="AV4" s="112"/>
-      <c r="AW4" s="112"/>
-      <c r="AX4" s="112"/>
-      <c r="AY4" s="112">
+      <c r="AS4" s="123"/>
+      <c r="AT4" s="123"/>
+      <c r="AU4" s="123"/>
+      <c r="AV4" s="123"/>
+      <c r="AW4" s="123"/>
+      <c r="AX4" s="123"/>
+      <c r="AY4" s="123">
         <f>AY5</f>
         <v>45327</v>
       </c>
-      <c r="AZ4" s="112"/>
-      <c r="BA4" s="112"/>
-      <c r="BB4" s="112"/>
-      <c r="BC4" s="112"/>
-      <c r="BD4" s="112"/>
-      <c r="BE4" s="112"/>
-      <c r="BF4" s="112">
+      <c r="AZ4" s="123"/>
+      <c r="BA4" s="123"/>
+      <c r="BB4" s="123"/>
+      <c r="BC4" s="123"/>
+      <c r="BD4" s="123"/>
+      <c r="BE4" s="123"/>
+      <c r="BF4" s="123">
         <f>BF5</f>
         <v>45334</v>
       </c>
-      <c r="BG4" s="112"/>
-      <c r="BH4" s="112"/>
-      <c r="BI4" s="112"/>
-      <c r="BJ4" s="112"/>
-      <c r="BK4" s="112"/>
-      <c r="BL4" s="113"/>
-    </row>
-    <row r="5" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="122"/>
-      <c r="B5" s="123" t="s">
+      <c r="BG4" s="123"/>
+      <c r="BH4" s="123"/>
+      <c r="BI4" s="123"/>
+      <c r="BJ4" s="123"/>
+      <c r="BK4" s="123"/>
+      <c r="BL4" s="124"/>
+    </row>
+    <row r="5" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="112"/>
+      <c r="B5" s="113" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="125" t="s">
+      <c r="C5" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="115" t="s">
+      <c r="D5" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="115" t="s">
+      <c r="E5" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="115" t="s">
+      <c r="F5" s="117" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="31">
@@ -2406,9 +2402,9 @@
         <v>45340</v>
       </c>
     </row>
-    <row r="6" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="122"/>
-      <c r="B6" s="124"/>
+    <row r="6" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="112"/>
+      <c r="B6" s="114"/>
       <c r="C6" s="116"/>
       <c r="D6" s="116"/>
       <c r="E6" s="116"/>
@@ -2638,7 +2634,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="7" spans="1:64" s="26" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:64" s="26" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="13" t="s">
         <v>20</v>
       </c>
@@ -2708,7 +2704,7 @@
       <c r="BK7" s="39"/>
       <c r="BL7" s="39"/>
     </row>
-    <row r="8" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="14"/>
       <c r="B8" s="40" t="s">
         <v>37</v>
@@ -2779,7 +2775,7 @@
       <c r="BK8" s="45"/>
       <c r="BL8" s="45"/>
     </row>
-    <row r="9" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="14"/>
       <c r="B9" s="104" t="s">
         <v>24</v>
@@ -2859,7 +2855,7 @@
       <c r="BK9" s="50"/>
       <c r="BL9" s="50"/>
     </row>
-    <row r="10" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="14"/>
       <c r="B10" s="105" t="s">
         <v>26</v>
@@ -2939,7 +2935,7 @@
       <c r="BK10" s="50"/>
       <c r="BL10" s="50"/>
     </row>
-    <row r="11" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="13"/>
       <c r="B11" s="106" t="s">
         <v>27</v>
@@ -3019,7 +3015,7 @@
       <c r="BK11" s="50"/>
       <c r="BL11" s="50"/>
     </row>
-    <row r="12" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="13"/>
       <c r="B12" s="107" t="s">
         <v>28</v>
@@ -3099,7 +3095,7 @@
       <c r="BK12" s="50"/>
       <c r="BL12" s="50"/>
     </row>
-    <row r="13" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="13"/>
       <c r="B13" s="51" t="s">
         <v>34</v>
@@ -3176,7 +3172,7 @@
       <c r="BK13" s="50"/>
       <c r="BL13" s="50"/>
     </row>
-    <row r="14" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="13"/>
       <c r="B14" s="107" t="s">
         <v>38</v>
@@ -3256,7 +3252,7 @@
       <c r="BK14" s="50"/>
       <c r="BL14" s="50"/>
     </row>
-    <row r="15" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="14"/>
       <c r="B15" s="56" t="s">
         <v>29</v>
@@ -3271,7 +3267,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="13"/>
       <c r="B16" s="108" t="s">
         <v>33</v>
@@ -3351,7 +3347,7 @@
       <c r="BK16" s="50"/>
       <c r="BL16" s="50"/>
     </row>
-    <row r="17" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="13"/>
       <c r="B17" s="64" t="s">
         <v>36</v>
@@ -3422,7 +3418,7 @@
       <c r="BK17" s="69"/>
       <c r="BL17" s="69"/>
     </row>
-    <row r="18" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="13"/>
       <c r="B18" s="109" t="s">
         <v>35</v>
@@ -3502,7 +3498,7 @@
       <c r="BK18" s="50"/>
       <c r="BL18" s="50"/>
     </row>
-    <row r="19" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="13"/>
       <c r="B19" s="110" t="s">
         <v>45</v>
@@ -3579,7 +3575,7 @@
       <c r="BK19" s="50"/>
       <c r="BL19" s="50"/>
     </row>
-    <row r="20" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="13"/>
       <c r="B20" s="110" t="s">
         <v>46</v>
@@ -3588,7 +3584,7 @@
         <v>39</v>
       </c>
       <c r="D20" s="72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="73">
         <v>45319</v>
@@ -3658,7 +3654,7 @@
       <c r="BK20" s="50"/>
       <c r="BL20" s="50"/>
     </row>
-    <row r="21" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="13"/>
       <c r="B21" s="70" t="s">
         <v>40</v>
@@ -3737,7 +3733,7 @@
       <c r="BK21" s="50"/>
       <c r="BL21" s="50"/>
     </row>
-    <row r="22" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="13"/>
       <c r="B22" s="74" t="s">
         <v>30</v>
@@ -3808,7 +3804,7 @@
       <c r="BK22" s="79"/>
       <c r="BL22" s="79"/>
     </row>
-    <row r="23" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="13"/>
       <c r="B23" s="111" t="s">
         <v>42</v>
@@ -3888,7 +3884,7 @@
       <c r="BK23" s="50"/>
       <c r="BL23" s="50"/>
     </row>
-    <row r="24" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="13"/>
       <c r="B24" s="111" t="s">
         <v>43</v>
@@ -3968,7 +3964,7 @@
       <c r="BK24" s="50"/>
       <c r="BL24" s="50"/>
     </row>
-    <row r="25" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="13"/>
       <c r="B25" s="111" t="s">
         <v>41</v>
@@ -4049,7 +4045,7 @@
       <c r="BK25" s="50"/>
       <c r="BL25" s="50"/>
     </row>
-    <row r="26" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="13"/>
       <c r="B26" s="80" t="s">
         <v>40</v>
@@ -4130,7 +4126,7 @@
       <c r="BK26" s="50"/>
       <c r="BL26" s="50"/>
     </row>
-    <row r="27" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="13"/>
       <c r="B27" s="84"/>
       <c r="C27" s="85"/>
@@ -4199,7 +4195,7 @@
       <c r="BK27" s="45"/>
       <c r="BL27" s="45"/>
     </row>
-    <row r="28" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="14"/>
       <c r="B28" s="88" t="s">
         <v>0</v>
@@ -4270,28 +4266,18 @@
       <c r="BK28" s="93"/>
       <c r="BL28" s="93"/>
     </row>
-    <row r="29" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C30" s="16"/>
       <c r="F30" s="15"/>
     </row>
-    <row r="31" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C31" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
@@ -4300,6 +4286,16 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <phoneticPr fontId="32" type="noConversion"/>
   <conditionalFormatting sqref="D7:D28">
@@ -4410,110 +4406,110 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="87" style="7" customWidth="1"/>
     <col min="2" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:2" s="9" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:2" s="9" customFormat="1" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A2" s="97" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:2" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="98"/>
       <c r="B3" s="12"/>
     </row>
-    <row r="4" spans="1:2" s="10" customFormat="1" ht="30.5" x14ac:dyDescent="0.85">
+    <row r="4" spans="1:2" s="10" customFormat="1" ht="31.3" x14ac:dyDescent="1.05">
       <c r="A4" s="99" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="100" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="99" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="7" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" s="7" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="101" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="10" customFormat="1" ht="30.5" x14ac:dyDescent="0.85">
+    <row r="8" spans="1:2" s="10" customFormat="1" ht="31.3" x14ac:dyDescent="1.05">
       <c r="A8" s="99" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="42" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="42.45" x14ac:dyDescent="0.3">
       <c r="A9" s="100" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="7" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" s="7" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="102" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="10" customFormat="1" ht="30.5" x14ac:dyDescent="0.85">
+    <row r="11" spans="1:2" s="10" customFormat="1" ht="31.3" x14ac:dyDescent="1.05">
       <c r="A11" s="99" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="28.3" x14ac:dyDescent="0.3">
       <c r="A12" s="100" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="7" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" s="7" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="102" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="10" customFormat="1" ht="30.5" x14ac:dyDescent="0.85">
+    <row r="14" spans="1:2" s="10" customFormat="1" ht="31.3" x14ac:dyDescent="1.05">
       <c r="A14" s="99" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="100" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="70" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="70.75" x14ac:dyDescent="0.3">
       <c r="A16" s="100" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="103"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="103"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="103"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="103"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="103"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="103"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="103"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="103"/>
     </row>
   </sheetData>
@@ -4550,6 +4546,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4861,15 +4866,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
@@ -4890,6 +4886,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2348D59-3426-404A-A0C5-6456F6613EDB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4910,14 +4914,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
add todo list and do some test
</commit_message>
<xml_diff>
--- a/Gantt_chart.xlsx
+++ b/Gantt_chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c680cefa49b2057/附件/程式1/Project/ytp-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="155" documentId="11_3C4179B01545E19DD6C385890107473B0B440F85" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62B13D6C-BA63-4EEA-BE1C-D882FE220A11}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="11_3C4179B01545E19DD6C385890107473B0B440F85" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51F2FCD2-696B-4DD4-A6F6-1E25F9551C32}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="754" yWindow="754" windowWidth="24686" windowHeight="13055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project schedule" sheetId="11" r:id="rId1"/>
@@ -1348,22 +1348,19 @@
     <xf numFmtId="0" fontId="36" fillId="10" borderId="9" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1375,14 +1372,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="179" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1776,6 +1776,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1984,8 +1988,8 @@
   </sheetPr>
   <dimension ref="A1:BL31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A10" zoomScale="106" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A16" zoomScale="106" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2011,28 +2015,28 @@
       <c r="E1" s="20"/>
       <c r="F1" s="21"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="121" t="s">
+      <c r="I1" s="120" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="122"/>
-      <c r="K1" s="122"/>
-      <c r="L1" s="122"/>
-      <c r="M1" s="122"/>
-      <c r="N1" s="122"/>
-      <c r="O1" s="122"/>
+      <c r="J1" s="121"/>
+      <c r="K1" s="121"/>
+      <c r="L1" s="121"/>
+      <c r="M1" s="121"/>
+      <c r="N1" s="121"/>
+      <c r="O1" s="121"/>
       <c r="P1" s="24"/>
-      <c r="Q1" s="120">
+      <c r="Q1" s="119">
         <v>45287</v>
       </c>
-      <c r="R1" s="119"/>
-      <c r="S1" s="119"/>
-      <c r="T1" s="119"/>
-      <c r="U1" s="119"/>
-      <c r="V1" s="119"/>
-      <c r="W1" s="119"/>
-      <c r="X1" s="119"/>
-      <c r="Y1" s="119"/>
-      <c r="Z1" s="119"/>
+      <c r="R1" s="118"/>
+      <c r="S1" s="118"/>
+      <c r="T1" s="118"/>
+      <c r="U1" s="118"/>
+      <c r="V1" s="118"/>
+      <c r="W1" s="118"/>
+      <c r="X1" s="118"/>
+      <c r="Y1" s="118"/>
+      <c r="Z1" s="118"/>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.8">
       <c r="B2" s="94" t="s">
@@ -2042,28 +2046,28 @@
       <c r="D2" s="22"/>
       <c r="E2" s="23"/>
       <c r="F2" s="22"/>
-      <c r="I2" s="121" t="s">
+      <c r="I2" s="120" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="122"/>
-      <c r="K2" s="122"/>
-      <c r="L2" s="122"/>
-      <c r="M2" s="122"/>
-      <c r="N2" s="122"/>
-      <c r="O2" s="122"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
+      <c r="N2" s="121"/>
+      <c r="O2" s="121"/>
       <c r="P2" s="24"/>
-      <c r="Q2" s="118">
+      <c r="Q2" s="117">
         <v>1</v>
       </c>
-      <c r="R2" s="119"/>
-      <c r="S2" s="119"/>
-      <c r="T2" s="119"/>
-      <c r="U2" s="119"/>
-      <c r="V2" s="119"/>
-      <c r="W2" s="119"/>
-      <c r="X2" s="119"/>
-      <c r="Y2" s="119"/>
-      <c r="Z2" s="119"/>
+      <c r="R2" s="118"/>
+      <c r="S2" s="118"/>
+      <c r="T2" s="118"/>
+      <c r="U2" s="118"/>
+      <c r="V2" s="118"/>
+      <c r="W2" s="118"/>
+      <c r="X2" s="118"/>
+      <c r="Y2" s="118"/>
+      <c r="Z2" s="118"/>
     </row>
     <row r="3" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
@@ -2079,102 +2083,102 @@
         <v>13</v>
       </c>
       <c r="E4" s="30"/>
-      <c r="I4" s="125">
+      <c r="I4" s="114">
         <f>I5</f>
         <v>45285</v>
       </c>
-      <c r="J4" s="123"/>
-      <c r="K4" s="123"/>
-      <c r="L4" s="123"/>
-      <c r="M4" s="123"/>
-      <c r="N4" s="123"/>
-      <c r="O4" s="123"/>
-      <c r="P4" s="123">
+      <c r="J4" s="112"/>
+      <c r="K4" s="112"/>
+      <c r="L4" s="112"/>
+      <c r="M4" s="112"/>
+      <c r="N4" s="112"/>
+      <c r="O4" s="112"/>
+      <c r="P4" s="112">
         <f>P5</f>
         <v>45292</v>
       </c>
-      <c r="Q4" s="123"/>
-      <c r="R4" s="123"/>
-      <c r="S4" s="123"/>
-      <c r="T4" s="123"/>
-      <c r="U4" s="123"/>
-      <c r="V4" s="123"/>
-      <c r="W4" s="123">
+      <c r="Q4" s="112"/>
+      <c r="R4" s="112"/>
+      <c r="S4" s="112"/>
+      <c r="T4" s="112"/>
+      <c r="U4" s="112"/>
+      <c r="V4" s="112"/>
+      <c r="W4" s="112">
         <f>W5</f>
         <v>45299</v>
       </c>
-      <c r="X4" s="123"/>
-      <c r="Y4" s="123"/>
-      <c r="Z4" s="123"/>
-      <c r="AA4" s="123"/>
-      <c r="AB4" s="123"/>
-      <c r="AC4" s="123"/>
-      <c r="AD4" s="123">
+      <c r="X4" s="112"/>
+      <c r="Y4" s="112"/>
+      <c r="Z4" s="112"/>
+      <c r="AA4" s="112"/>
+      <c r="AB4" s="112"/>
+      <c r="AC4" s="112"/>
+      <c r="AD4" s="112">
         <f>AD5</f>
         <v>45306</v>
       </c>
-      <c r="AE4" s="123"/>
-      <c r="AF4" s="123"/>
-      <c r="AG4" s="123"/>
-      <c r="AH4" s="123"/>
-      <c r="AI4" s="123"/>
-      <c r="AJ4" s="123"/>
-      <c r="AK4" s="123">
+      <c r="AE4" s="112"/>
+      <c r="AF4" s="112"/>
+      <c r="AG4" s="112"/>
+      <c r="AH4" s="112"/>
+      <c r="AI4" s="112"/>
+      <c r="AJ4" s="112"/>
+      <c r="AK4" s="112">
         <f>AK5</f>
         <v>45313</v>
       </c>
-      <c r="AL4" s="123"/>
-      <c r="AM4" s="123"/>
-      <c r="AN4" s="123"/>
-      <c r="AO4" s="123"/>
-      <c r="AP4" s="123"/>
-      <c r="AQ4" s="123"/>
-      <c r="AR4" s="123">
+      <c r="AL4" s="112"/>
+      <c r="AM4" s="112"/>
+      <c r="AN4" s="112"/>
+      <c r="AO4" s="112"/>
+      <c r="AP4" s="112"/>
+      <c r="AQ4" s="112"/>
+      <c r="AR4" s="112">
         <f>AR5</f>
         <v>45320</v>
       </c>
-      <c r="AS4" s="123"/>
-      <c r="AT4" s="123"/>
-      <c r="AU4" s="123"/>
-      <c r="AV4" s="123"/>
-      <c r="AW4" s="123"/>
-      <c r="AX4" s="123"/>
-      <c r="AY4" s="123">
+      <c r="AS4" s="112"/>
+      <c r="AT4" s="112"/>
+      <c r="AU4" s="112"/>
+      <c r="AV4" s="112"/>
+      <c r="AW4" s="112"/>
+      <c r="AX4" s="112"/>
+      <c r="AY4" s="112">
         <f>AY5</f>
         <v>45327</v>
       </c>
-      <c r="AZ4" s="123"/>
-      <c r="BA4" s="123"/>
-      <c r="BB4" s="123"/>
-      <c r="BC4" s="123"/>
-      <c r="BD4" s="123"/>
-      <c r="BE4" s="123"/>
-      <c r="BF4" s="123">
+      <c r="AZ4" s="112"/>
+      <c r="BA4" s="112"/>
+      <c r="BB4" s="112"/>
+      <c r="BC4" s="112"/>
+      <c r="BD4" s="112"/>
+      <c r="BE4" s="112"/>
+      <c r="BF4" s="112">
         <f>BF5</f>
         <v>45334</v>
       </c>
-      <c r="BG4" s="123"/>
-      <c r="BH4" s="123"/>
-      <c r="BI4" s="123"/>
-      <c r="BJ4" s="123"/>
-      <c r="BK4" s="123"/>
-      <c r="BL4" s="124"/>
+      <c r="BG4" s="112"/>
+      <c r="BH4" s="112"/>
+      <c r="BI4" s="112"/>
+      <c r="BJ4" s="112"/>
+      <c r="BK4" s="112"/>
+      <c r="BL4" s="113"/>
     </row>
     <row r="5" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="112"/>
-      <c r="B5" s="113" t="s">
+      <c r="A5" s="122"/>
+      <c r="B5" s="123" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="115" t="s">
+      <c r="C5" s="125" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="117" t="s">
+      <c r="D5" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="117" t="s">
+      <c r="E5" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="117" t="s">
+      <c r="F5" s="115" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="31">
@@ -2403,8 +2407,8 @@
       </c>
     </row>
     <row r="6" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="112"/>
-      <c r="B6" s="114"/>
+      <c r="A6" s="122"/>
+      <c r="B6" s="124"/>
       <c r="C6" s="116"/>
       <c r="D6" s="116"/>
       <c r="E6" s="116"/>
@@ -3813,7 +3817,7 @@
         <v>25</v>
       </c>
       <c r="D23" s="82">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E23" s="83">
         <v>45308</v>
@@ -3973,7 +3977,7 @@
         <v>39</v>
       </c>
       <c r="D25" s="82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="83">
         <f>E23+7</f>
@@ -4278,6 +4282,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
@@ -4286,16 +4300,6 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <phoneticPr fontId="32" type="noConversion"/>
   <conditionalFormatting sqref="D7:D28">
@@ -4526,35 +4530,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4866,34 +4841,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2348D59-3426-404A-A0C5-6456F6613EDB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4914,6 +4891,33 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>